<commit_message>
Poniendo mejor las combinaciones unicas mucho mejor para mejorar la integridad de los datos y mejorando las descripciones de cada objeto y atributos de conjuntos residenciales, residentes y solo la mitad de agendas
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Modelos de Dominio Enriquecidos/Modelo De Dominio Enriquecido Agendas.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Modelos de Dominio Enriquecidos/Modelo De Dominio Enriquecido Agendas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Nueva Version Victus/Modelos de Dominio Enriquecidos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Nueva Version Victus\Modelos de Dominio Enriquecidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38D7C069-303E-47B5-A35C-4342BE7821F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC346671-86C7-4639-9E1C-1C0B79FC1C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{9E75F319-B909-453D-9AFC-FA9C5B40B20E}"/>
+    <workbookView xWindow="-396" yWindow="3624" windowWidth="17280" windowHeight="8880" firstSheet="3" activeTab="3" xr2:uid="{9E75F319-B909-453D-9AFC-FA9C5B40B20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="Agenda" sheetId="5" r:id="rId5"/>
     <sheet name="Turno" sheetId="6" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1328,7 +1331,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="121">
   <si>
     <t>Tipo Objeto Dominio</t>
   </si>
@@ -1546,12 +1549,6 @@
     <t>descripcion</t>
   </si>
   <si>
-    <t>capacidad</t>
-  </si>
-  <si>
-    <t>tiempoUsoDia</t>
-  </si>
-  <si>
     <t>normas</t>
   </si>
   <si>
@@ -1685,6 +1682,18 @@
   </si>
   <si>
     <t xml:space="preserve">agenda </t>
+  </si>
+  <si>
+    <t>capacidadPersonas</t>
+  </si>
+  <si>
+    <t>tiempoUso</t>
+  </si>
+  <si>
+    <t>unidadTiempoUso</t>
+  </si>
+  <si>
+    <t>ConjuntoResidencial</t>
   </si>
 </sst>
 </file>
@@ -2165,12 +2174,6 @@
   </cellStyleXfs>
   <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2184,279 +2187,285 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2538,8 +2547,40 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Objetos de dominio"/>
+      <sheetName val="Administrador"/>
+      <sheetName val="ConjuntoResidencial"/>
+      <sheetName val="Zonainmueble"/>
+      <sheetName val="Inmueble"/>
+      <sheetName val="ZonaComun"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5">
+        <row r="2">
+          <cell r="G2" t="str">
+            <v>Es un dato que representa la unidad de tiempo de uso de una zona comun para un residente.</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2861,89 +2902,89 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="60"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2961,7 +3002,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2976,77 +3017,77 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.44140625" style="12"/>
+    <col min="1" max="1" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="62"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="19" t="str">
+      <c r="D3" s="63" t="str">
         <f>$B$1</f>
         <v>Agendas</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="21"/>
+      <c r="D4" s="64"/>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="20"/>
+      <c r="D5" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3064,731 +3105,779 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BC2B36-176F-457B-9E5A-2C1354FBA2A7}">
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.33203125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="79.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="12"/>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="93"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="24" t="str">
+      <c r="B2" s="94" t="str">
         <f>'Listado Objetos de Dominio'!A3</f>
         <v>ZonaComun</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="94"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="25" t="str">
+      <c r="B3" s="95" t="str">
         <f>'Listado Objetos de Dominio'!B3</f>
         <v>Objeto de dominio que representa a cada una de las zonas comúnes que tendrán una agenda y respectivos turnos.</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="27" t="s">
+      <c r="O4" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="P4" s="27" t="s">
+      <c r="P4" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" s="28" t="s">
+      <c r="Q4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="29" t="str">
-        <f>A20</f>
+      <c r="R4" s="19" t="str">
+        <f>A21</f>
         <v>Reponsabilidad 1</v>
       </c>
-      <c r="S4" s="30" t="str">
-        <f>A21</f>
+      <c r="S4" s="20" t="str">
+        <f>A22</f>
         <v>Reponsabilidad 2</v>
       </c>
-      <c r="T4" s="31" t="str">
-        <f>A22</f>
+      <c r="T4" s="21" t="str">
+        <f>A23</f>
         <v>Reponsabilidad 3</v>
       </c>
-      <c r="U4" s="32" t="str">
-        <f>A23</f>
+      <c r="U4" s="22" t="str">
+        <f>A24</f>
         <v>Reponsabilidad 4</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="23">
         <v>32</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="23">
         <v>32</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34" t="s">
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="J5" s="33"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="36" t="s">
+      <c r="J5" s="23"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="M5" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N5" s="33" t="s">
+      <c r="M5" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="O5" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="P5" s="33" t="s">
+      <c r="O5" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="Q5" s="34" t="s">
+      <c r="Q5" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="R5" s="37"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="40"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="30"/>
     </row>
     <row r="6" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="23">
         <v>1</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="23">
         <v>50</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="34" t="s">
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="35" t="s">
+      <c r="J6" s="23"/>
+      <c r="K6" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P6" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="L6" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N6" s="33" t="s">
+      <c r="R6" s="27"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="30"/>
+    </row>
+    <row r="7" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="23">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23">
+        <v>50</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="23"/>
+      <c r="K7" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="P6" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q6" s="34" t="s">
+      <c r="O7" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="P7" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q7" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="R7" s="27"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="30"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N8" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="O8" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q8" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="R6" s="37"/>
-      <c r="S6" s="38"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="40"/>
-    </row>
-    <row r="7" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="33" t="s">
+      <c r="R8" s="27"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="30"/>
+    </row>
+    <row r="9" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9" s="23"/>
+      <c r="K9" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="O9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q9" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="R9" s="27"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="30"/>
+    </row>
+    <row r="10" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C10" s="23">
         <v>1</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D10" s="23">
         <v>50</v>
       </c>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34" t="s">
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="33"/>
-      <c r="K7" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="L7" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="M7" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N7" s="33" t="s">
+      <c r="J10" s="23"/>
+      <c r="K10" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N10" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="33" t="s">
+      <c r="O10" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P10" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q10" s="24" t="str">
+        <f>[1]ZonaComun!$G$2</f>
+        <v>Es un dato que representa la unidad de tiempo de uso de una zona comun para un residente.</v>
+      </c>
+      <c r="R10" s="27"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="30"/>
+    </row>
+    <row r="11" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="23">
+        <v>1</v>
+      </c>
+      <c r="D11" s="23">
+        <v>5000</v>
+      </c>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="23"/>
+      <c r="K11" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="M11" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N11" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="P7" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q7" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="R7" s="37"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="40"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N8" s="33" t="s">
+      <c r="O11" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="O8" s="33" t="s">
+      <c r="P11" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q11" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="R11" s="27"/>
+      <c r="S11" s="28"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="30"/>
+    </row>
+    <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="P8" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q8" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="R8" s="37"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="40"/>
-    </row>
-    <row r="9" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="41" t="s">
+      <c r="M12" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="O12" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P12" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q12" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="R12" s="27"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="30"/>
+    </row>
+    <row r="13" spans="1:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="90" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="91"/>
+      <c r="C14" s="92"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="84" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="86" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="85"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="J9" s="33"/>
-      <c r="K9" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="L9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="M9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="O9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="P9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q9" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="R9" s="37"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="39"/>
-      <c r="U9" s="40"/>
-    </row>
-    <row r="10" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="33">
-        <v>1</v>
-      </c>
-      <c r="D10" s="33">
-        <v>5000</v>
-      </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="J10" s="33"/>
-      <c r="K10" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="L10" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="M10" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N10" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="O10" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="P10" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q10" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="R10" s="37"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="39"/>
-      <c r="U10" s="40"/>
-    </row>
-    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="95" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="M11" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N11" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="O11" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="P11" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q11" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="R11" s="37"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="39"/>
-      <c r="U11" s="40"/>
-    </row>
-    <row r="12" spans="1:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="44"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="46" t="s">
+    </row>
+    <row r="18" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="88" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="47" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="50" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="52"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="54" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56" t="s">
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19" s="78"/>
+      <c r="M19" s="78"/>
+      <c r="N19" s="78"/>
+      <c r="O19" s="78"/>
+      <c r="P19" s="78" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q19" s="78"/>
+      <c r="R19" s="78" t="s">
+        <v>63</v>
+      </c>
+      <c r="S19" s="79"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="89"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="56"/>
-      <c r="O18" s="56"/>
-      <c r="P18" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q18" s="56"/>
-      <c r="R18" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="S18" s="57"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="58"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="60" t="s">
-        <v>64</v>
-      </c>
-      <c r="I19" s="60" t="s">
-        <v>65</v>
-      </c>
-      <c r="J19" s="60" t="s">
+      <c r="K20" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="L20" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="K19" s="60" t="s">
-        <v>31</v>
-      </c>
-      <c r="L19" s="59" t="s">
+      <c r="M20" s="80"/>
+      <c r="N20" s="80"/>
+      <c r="O20" s="80"/>
+      <c r="P20" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q20" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="M19" s="59"/>
-      <c r="N19" s="59"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="60" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q19" s="60" t="s">
-        <v>2</v>
-      </c>
-      <c r="R19" s="60" t="s">
+      <c r="R20" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="S19" s="61" t="s">
+      <c r="S20" s="38" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="62" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="64"/>
-      <c r="N20" s="64"/>
-      <c r="O20" s="64"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="65"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="66" t="s">
+      <c r="B21" s="82"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="83"/>
+      <c r="M21" s="83"/>
+      <c r="N21" s="83"/>
+      <c r="O21" s="83"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="39"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="67"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="70"/>
-      <c r="J21" s="71"/>
-      <c r="K21" s="72"/>
-      <c r="L21" s="73"/>
-      <c r="M21" s="73"/>
-      <c r="N21" s="73"/>
-      <c r="O21" s="73"/>
-      <c r="P21" s="38"/>
-      <c r="Q21" s="74"/>
-      <c r="R21" s="74"/>
-      <c r="S21" s="75"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="76" t="s">
+      <c r="B22" s="71"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="73"/>
+      <c r="N22" s="73"/>
+      <c r="O22" s="73"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="44"/>
+      <c r="R22" s="44"/>
+      <c r="S22" s="45"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="77"/>
-      <c r="C22" s="78"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="82"/>
-      <c r="L22" s="83"/>
-      <c r="M22" s="83"/>
-      <c r="N22" s="83"/>
-      <c r="O22" s="83"/>
-      <c r="P22" s="39"/>
-      <c r="Q22" s="84"/>
-      <c r="R22" s="84"/>
-      <c r="S22" s="85"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="86" t="s">
+      <c r="B23" s="75"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="77"/>
+      <c r="M23" s="77"/>
+      <c r="N23" s="77"/>
+      <c r="O23" s="77"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="50"/>
+      <c r="S23" s="51"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="87"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="89"/>
-      <c r="I23" s="90"/>
-      <c r="J23" s="91"/>
-      <c r="K23" s="89"/>
-      <c r="L23" s="92"/>
-      <c r="M23" s="92"/>
-      <c r="N23" s="92"/>
-      <c r="O23" s="92"/>
-      <c r="P23" s="40"/>
-      <c r="Q23" s="93"/>
-      <c r="R23" s="93"/>
-      <c r="S23" s="94"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="69"/>
+      <c r="N24" s="69"/>
+      <c r="O24" s="69"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="55"/>
+      <c r="R24" s="55"/>
+      <c r="S24" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A19:B20"/>
+    <mergeCell ref="C19:G20"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="K19:O19"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="L22:O22"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="L23:O23"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="L19:O19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C18:G19"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:O18"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:Q3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{A37B2855-ACFA-479C-B06A-FD8440512F11}"/>
-    <hyperlink ref="I23" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{F13992CF-F5F1-4DDC-A387-BCD26ACFBC51}"/>
+    <hyperlink ref="I24" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{F13992CF-F5F1-4DDC-A387-BCD26ACFBC51}"/>
     <hyperlink ref="S4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{0EC11F90-A79E-4B65-9D18-7458195FFCB3}"/>
     <hyperlink ref="T4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{F13F5B8F-A470-43A8-B18B-490DB3960315}"/>
     <hyperlink ref="U4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{79C534C1-4DBB-44B7-91DC-673B55BE9C76}"/>
-    <hyperlink ref="A21:B21" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{73E8B593-130A-4B51-B491-CBA9818A5291}"/>
-    <hyperlink ref="A20:B20" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{ADFBCBA3-21F7-4DAC-9323-C82903924B4C}"/>
-    <hyperlink ref="A23:B23" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{9B7049B6-504E-4D10-B27F-B6F6A55662CB}"/>
+    <hyperlink ref="A22:B22" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{73E8B593-130A-4B51-B491-CBA9818A5291}"/>
+    <hyperlink ref="A21:B21" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{ADFBCBA3-21F7-4DAC-9323-C82903924B4C}"/>
+    <hyperlink ref="A24:B24" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{9B7049B6-504E-4D10-B27F-B6F6A55662CB}"/>
     <hyperlink ref="R4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{E3D4DA29-2AA5-4D85-86F9-7BF7982D8569}"/>
     <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{E623D929-425F-430D-84C6-20E89FCA63A8}"/>
-    <hyperlink ref="A22:B22" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{996910C1-B38D-4573-9988-E75C7389CC3A}"/>
+    <hyperlink ref="A23:B23" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{996910C1-B38D-4573-9988-E75C7389CC3A}"/>
     <hyperlink ref="A5" location="Residente!A12" display="identificador" xr:uid="{0A4FCE87-A9CF-4ED7-8769-A328C8D230AE}"/>
-    <hyperlink ref="C15" location="ZonaComun!A6" display="nombre" xr:uid="{1917D422-53D3-4E12-84AE-0BAFFA848476}"/>
-    <hyperlink ref="C16" location="ZonaComun!A11" display="conjuntoResidencial" xr:uid="{A1BD3261-AA24-49AC-80D8-B62D3C3ECFE9}"/>
+    <hyperlink ref="C16" location="ZonaComun!A6" display="nombre" xr:uid="{1917D422-53D3-4E12-84AE-0BAFFA848476}"/>
+    <hyperlink ref="C17" location="ZonaComun!A11" display="conjuntoResidencial" xr:uid="{A1BD3261-AA24-49AC-80D8-B62D3C3ECFE9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3803,664 +3892,647 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.33203125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="79.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="12"/>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="93"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="24" t="str">
+      <c r="B2" s="94" t="str">
         <f>'Listado Objetos de Dominio'!A4</f>
         <v>Agenda</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="94"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="25" t="str">
+      <c r="B3" s="95" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representaa cada una de las agendas que dónde el residente podrá reservar.</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="27" t="s">
+      <c r="O4" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="P4" s="27" t="s">
+      <c r="P4" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" s="28" t="s">
+      <c r="Q4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="29" t="str">
+      <c r="R4" s="19" t="str">
         <f>A21</f>
         <v>Reponsabilidad 1</v>
       </c>
-      <c r="S4" s="30" t="str">
+      <c r="S4" s="20" t="str">
         <f>A22</f>
         <v>Reponsabilidad 2</v>
       </c>
-      <c r="T4" s="31" t="str">
+      <c r="T4" s="21" t="str">
         <f>A23</f>
         <v>Reponsabilidad 3</v>
       </c>
-      <c r="U4" s="32" t="str">
+      <c r="U4" s="22" t="str">
         <f>A24</f>
         <v>Reponsabilidad 4</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="23">
         <v>32</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="23">
         <v>32</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34" t="s">
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="O5" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q5" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="J5" s="33"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="36" t="s">
+      <c r="R5" s="27"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="30"/>
+    </row>
+    <row r="6" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="23">
+        <v>1</v>
+      </c>
+      <c r="D6" s="23">
+        <v>50</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" s="23"/>
+      <c r="K6" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="M5" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N5" s="33" t="s">
+      <c r="O6" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P6" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="R6" s="27"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="30"/>
+    </row>
+    <row r="7" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="23"/>
+      <c r="K7" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="O5" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="P5" s="33" t="s">
+      <c r="O7" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P7" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q7" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="R7" s="27"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="30"/>
+    </row>
+    <row r="8" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N8" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="Q5" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="R5" s="37"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="40"/>
-    </row>
-    <row r="6" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="33">
-        <v>1</v>
-      </c>
-      <c r="D6" s="33">
-        <v>50</v>
-      </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="34" t="s">
+      <c r="O8" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q8" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="R8" s="27"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="30"/>
+    </row>
+    <row r="9" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="35" t="s">
+      <c r="J9" s="23"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N9" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="O9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q9" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="R9" s="27"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="30"/>
+    </row>
+    <row r="10" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="L6" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N6" s="33" t="s">
+      <c r="L10" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N10" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="P6" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q6" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="R6" s="37"/>
-      <c r="S6" s="38"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="40"/>
-    </row>
-    <row r="7" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="J7" s="33"/>
-      <c r="K7" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="L7" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="M7" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N7" s="33" t="s">
+      <c r="O10" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="P7" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q7" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="R7" s="37"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="40"/>
-    </row>
-    <row r="8" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N8" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="O8" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="P8" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q8" s="34" t="s">
+      <c r="P10" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q10" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="R8" s="37"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="40"/>
-    </row>
-    <row r="9" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="J9" s="33"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="M9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N9" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="O9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="P9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q9" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="R9" s="37"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="39"/>
-      <c r="U9" s="40"/>
-    </row>
-    <row r="10" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="L10" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="M10" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N10" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="O10" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="P10" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q10" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="R10" s="37"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="39"/>
-      <c r="U10" s="40"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="30"/>
     </row>
     <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="44"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="92"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="34" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="97" t="s">
-        <v>104</v>
-      </c>
-      <c r="B14" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="50" t="s">
+      <c r="A14" s="96" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="86" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="35" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="98"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="50" t="s">
+      <c r="A15" s="97"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="97"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="98"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="58" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="98"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="50" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="99"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="96" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56" t="s">
+      <c r="B19" s="78"/>
+      <c r="C19" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56" t="s">
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56" t="s">
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="56"/>
-      <c r="P19" s="56" t="s">
+      <c r="L19" s="78"/>
+      <c r="M19" s="78"/>
+      <c r="N19" s="78"/>
+      <c r="O19" s="78"/>
+      <c r="P19" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="Q19" s="56"/>
-      <c r="R19" s="56" t="s">
+      <c r="Q19" s="78"/>
+      <c r="R19" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="S19" s="57"/>
+      <c r="S19" s="79"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="58"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="60" t="s">
+      <c r="A20" s="89"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="I20" s="60" t="s">
+      <c r="I20" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="J20" s="60" t="s">
+      <c r="J20" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="K20" s="60" t="s">
+      <c r="K20" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="L20" s="59" t="s">
+      <c r="L20" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="59"/>
-      <c r="N20" s="59"/>
-      <c r="O20" s="59"/>
-      <c r="P20" s="60" t="s">
+      <c r="M20" s="80"/>
+      <c r="N20" s="80"/>
+      <c r="O20" s="80"/>
+      <c r="P20" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="Q20" s="60" t="s">
+      <c r="Q20" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="R20" s="60" t="s">
+      <c r="R20" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="S20" s="61" t="s">
+      <c r="S20" s="38" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="62" t="s">
+      <c r="A21" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="64"/>
-      <c r="N21" s="64"/>
-      <c r="O21" s="64"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="65"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="83"/>
+      <c r="M21" s="83"/>
+      <c r="N21" s="83"/>
+      <c r="O21" s="83"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="39"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="67"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="72"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="43"/>
       <c r="L22" s="73"/>
       <c r="M22" s="73"/>
       <c r="N22" s="73"/>
       <c r="O22" s="73"/>
-      <c r="P22" s="38"/>
-      <c r="Q22" s="74"/>
-      <c r="R22" s="74"/>
-      <c r="S22" s="75"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="44"/>
+      <c r="R22" s="44"/>
+      <c r="S22" s="45"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="76" t="s">
+      <c r="A23" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="77"/>
-      <c r="C23" s="78"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="81"/>
-      <c r="K23" s="82"/>
-      <c r="L23" s="83"/>
-      <c r="M23" s="83"/>
-      <c r="N23" s="83"/>
-      <c r="O23" s="83"/>
-      <c r="P23" s="39"/>
-      <c r="Q23" s="84"/>
-      <c r="R23" s="84"/>
-      <c r="S23" s="85"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="77"/>
+      <c r="M23" s="77"/>
+      <c r="N23" s="77"/>
+      <c r="O23" s="77"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="50"/>
+      <c r="S23" s="51"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="86" t="s">
+      <c r="A24" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="87"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="89"/>
-      <c r="I24" s="90"/>
-      <c r="J24" s="91"/>
-      <c r="K24" s="89"/>
-      <c r="L24" s="92"/>
-      <c r="M24" s="92"/>
-      <c r="N24" s="92"/>
-      <c r="O24" s="92"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="93"/>
-      <c r="R24" s="93"/>
-      <c r="S24" s="94"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="69"/>
+      <c r="N24" s="69"/>
+      <c r="O24" s="69"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="55"/>
+      <c r="R24" s="55"/>
+      <c r="S24" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="A19:B20"/>
-    <mergeCell ref="C19:G20"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:O19"/>
-    <mergeCell ref="P19:Q19"/>
     <mergeCell ref="R19:S19"/>
     <mergeCell ref="L20:O20"/>
     <mergeCell ref="A1:Q1"/>
@@ -4469,6 +4541,23 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A19:B20"/>
+    <mergeCell ref="C19:G20"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:O19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="L24:O24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{B2E38F92-070F-4A08-9587-748CDC5E3622}"/>
@@ -4495,664 +4584,647 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC57795F-B02D-497B-A04E-44BC1D3D4128}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.33203125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="79.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="12"/>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="93"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="24" t="str">
+      <c r="B2" s="94" t="str">
         <f>'Listado Objetos de Dominio'!A4</f>
         <v>Agenda</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="94"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="25" t="str">
+      <c r="B3" s="95" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representaa cada una de las agendas que dónde el residente podrá reservar.</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="27" t="s">
+      <c r="O4" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="P4" s="27" t="s">
+      <c r="P4" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" s="28" t="s">
+      <c r="Q4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="29" t="str">
+      <c r="R4" s="19" t="str">
         <f>A21</f>
         <v>Reponsabilidad 1</v>
       </c>
-      <c r="S4" s="30" t="str">
+      <c r="S4" s="20" t="str">
         <f>A22</f>
         <v>Reponsabilidad 2</v>
       </c>
-      <c r="T4" s="31" t="str">
+      <c r="T4" s="21" t="str">
         <f>A23</f>
         <v>Reponsabilidad 3</v>
       </c>
-      <c r="U4" s="32" t="str">
+      <c r="U4" s="22" t="str">
         <f>A24</f>
         <v>Reponsabilidad 4</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="23">
         <v>32</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="23">
         <v>32</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="J5" s="33"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="36" t="s">
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="M5" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N5" s="33" t="s">
+      <c r="M5" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="O5" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="P5" s="33" t="s">
+      <c r="O5" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="Q5" s="34" t="s">
+      <c r="Q5" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="R5" s="27"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="30"/>
+    </row>
+    <row r="6" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="R5" s="37"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="40"/>
-    </row>
-    <row r="6" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="41" t="s">
+      <c r="B6" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="23">
+        <v>1</v>
+      </c>
+      <c r="D6" s="23">
+        <v>50</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" s="23"/>
+      <c r="K6" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P6" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="R6" s="27"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="30"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="23"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="O7" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P7" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q7" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="R7" s="27"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="30"/>
+    </row>
+    <row r="8" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N8" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="O8" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q8" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="33">
-        <v>1</v>
-      </c>
-      <c r="D6" s="33">
-        <v>50</v>
-      </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="34" t="s">
+      <c r="R8" s="27"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="30"/>
+    </row>
+    <row r="9" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="L6" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N6" s="33" t="s">
+      <c r="J9" s="23"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N9" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="P6" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q6" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="R6" s="37"/>
-      <c r="S6" s="38"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="40"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="J7" s="33"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="M7" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N7" s="33" t="s">
+      <c r="O9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q9" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="R9" s="27"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="30"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N10" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="P7" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q7" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="R7" s="37"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="40"/>
-    </row>
-    <row r="8" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N8" s="33" t="s">
+      <c r="O10" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="O8" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="P8" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q8" s="34" t="s">
+      <c r="P10" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q10" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="R8" s="37"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="40"/>
-    </row>
-    <row r="9" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="J9" s="33"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="M9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N9" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="O9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="P9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q9" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="R9" s="37"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="39"/>
-      <c r="U9" s="40"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="M10" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N10" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="O10" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="P10" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q10" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="R10" s="37"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="39"/>
-      <c r="U10" s="40"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="30"/>
     </row>
     <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="44"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="92"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="34" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="97" t="s">
+      <c r="A14" s="96" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="86" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="97"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="97"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="35" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="98"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="58" t="s">
         <v>116</v>
-      </c>
-      <c r="B14" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" s="50" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="98"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="50" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="98"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="50" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="99"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="96" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56" t="s">
+      <c r="B19" s="78"/>
+      <c r="C19" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56" t="s">
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56" t="s">
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="56"/>
-      <c r="P19" s="56" t="s">
+      <c r="L19" s="78"/>
+      <c r="M19" s="78"/>
+      <c r="N19" s="78"/>
+      <c r="O19" s="78"/>
+      <c r="P19" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="Q19" s="56"/>
-      <c r="R19" s="56" t="s">
+      <c r="Q19" s="78"/>
+      <c r="R19" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="S19" s="57"/>
+      <c r="S19" s="79"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="58"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="60" t="s">
+      <c r="A20" s="89"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="I20" s="60" t="s">
+      <c r="I20" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="J20" s="60" t="s">
+      <c r="J20" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="K20" s="60" t="s">
+      <c r="K20" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="L20" s="59" t="s">
+      <c r="L20" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="59"/>
-      <c r="N20" s="59"/>
-      <c r="O20" s="59"/>
-      <c r="P20" s="60" t="s">
+      <c r="M20" s="80"/>
+      <c r="N20" s="80"/>
+      <c r="O20" s="80"/>
+      <c r="P20" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="Q20" s="60" t="s">
+      <c r="Q20" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="R20" s="60" t="s">
+      <c r="R20" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="S20" s="61" t="s">
+      <c r="S20" s="38" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="62" t="s">
+      <c r="A21" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="64"/>
-      <c r="N21" s="64"/>
-      <c r="O21" s="64"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="65"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="83"/>
+      <c r="M21" s="83"/>
+      <c r="N21" s="83"/>
+      <c r="O21" s="83"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="39"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="67"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="72"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="43"/>
       <c r="L22" s="73"/>
       <c r="M22" s="73"/>
       <c r="N22" s="73"/>
       <c r="O22" s="73"/>
-      <c r="P22" s="38"/>
-      <c r="Q22" s="74"/>
-      <c r="R22" s="74"/>
-      <c r="S22" s="75"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="44"/>
+      <c r="R22" s="44"/>
+      <c r="S22" s="45"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="76" t="s">
+      <c r="A23" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="77"/>
-      <c r="C23" s="78"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="81"/>
-      <c r="K23" s="82"/>
-      <c r="L23" s="83"/>
-      <c r="M23" s="83"/>
-      <c r="N23" s="83"/>
-      <c r="O23" s="83"/>
-      <c r="P23" s="39"/>
-      <c r="Q23" s="84"/>
-      <c r="R23" s="84"/>
-      <c r="S23" s="85"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="77"/>
+      <c r="M23" s="77"/>
+      <c r="N23" s="77"/>
+      <c r="O23" s="77"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="50"/>
+      <c r="S23" s="51"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="86" t="s">
+      <c r="A24" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="87"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="89"/>
-      <c r="I24" s="90"/>
-      <c r="J24" s="91"/>
-      <c r="K24" s="89"/>
-      <c r="L24" s="92"/>
-      <c r="M24" s="92"/>
-      <c r="N24" s="92"/>
-      <c r="O24" s="92"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="93"/>
-      <c r="R24" s="93"/>
-      <c r="S24" s="94"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="69"/>
+      <c r="N24" s="69"/>
+      <c r="O24" s="69"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="55"/>
+      <c r="R24" s="55"/>
+      <c r="S24" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="A19:B20"/>
-    <mergeCell ref="C19:G20"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:O19"/>
-    <mergeCell ref="P19:Q19"/>
     <mergeCell ref="R19:S19"/>
     <mergeCell ref="L20:O20"/>
     <mergeCell ref="A1:Q1"/>
@@ -5161,6 +5233,23 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A19:B20"/>
+    <mergeCell ref="C19:G20"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:O19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="L24:O24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{186E73A2-C89F-4A82-8727-EBDE505719F2}"/>

</xml_diff>

<commit_message>
Correcciones al muestreo de datos y el modelo enriquesido de agenda
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Modelos de Dominio Enriquecidos/Modelo De Dominio Enriquecido Agendas.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Modelos de Dominio Enriquecidos/Modelo De Dominio Enriquecido Agendas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Nueva Version Victus\Modelos de Dominio Enriquecidos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josez\Documents\Universidad IngeSistemas\Diseño Orientado a Objetos(DOO)\VictusProyect\victus-doc\Doo-Doc\Nueva Version Victus\Modelos de Dominio Enriquecidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC346671-86C7-4639-9E1C-1C0B79FC1C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A008BD63-2E2D-4E82-97FA-DCA88F8CD5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-396" yWindow="3624" windowWidth="17280" windowHeight="8880" firstSheet="3" activeTab="3" xr2:uid="{9E75F319-B909-453D-9AFC-FA9C5B40B20E}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="3" activeTab="5" xr2:uid="{9E75F319-B909-453D-9AFC-FA9C5B40B20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
     <author>Usuario 207</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{1AC144B8-4469-4DB7-9486-708F07AA540A}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{AA650CDA-91A2-402B-8E7D-83571F72C595}">
       <text>
         <r>
           <rPr>
@@ -73,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{DCBE8D51-D2EC-4ADE-8C2B-BAD7A5A5B989}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{7A5CBF73-0C22-4BF5-9215-A9302F403C4D}">
       <text>
         <r>
           <rPr>
@@ -104,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{640656D3-49FF-41B2-A15A-2B73FC499345}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{38454CF1-1423-43FB-91B1-D34C2EBF7B8E}">
       <text>
         <r>
           <rPr>
@@ -128,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{C5870276-1824-4C70-B6B2-0E02B74DC8A8}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{66DEFC34-855A-4FF0-A570-080940B2FB29}">
       <text>
         <r>
           <rPr>
@@ -153,7 +153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{AF9B424C-85EE-492E-BB53-70EBF3BBC229}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{6AECA2EC-0AE2-4A3A-B993-EAA893F14574}">
       <text>
         <r>
           <rPr>
@@ -177,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{261FCD4C-5D44-4C19-B721-8779E3BDB9AE}">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{4807D05E-92A9-4350-BC8E-B58EAE8338C4}">
       <text>
         <r>
           <rPr>
@@ -203,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{F830DBF7-67B1-4DC1-8BB8-9EABFECF88F7}">
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{C012051F-826D-4F27-AD87-9528CF359CA0}">
       <text>
         <r>
           <rPr>
@@ -227,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{353AF5DA-1C28-43BC-A162-4F1BA281672D}">
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{ED5D7D5B-3FF8-4C5E-8AA0-345DA9BFC19B}">
       <text>
         <r>
           <rPr>
@@ -252,7 +252,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{0CEA8030-3803-4E03-8615-95AE755CE1AD}">
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{8AFB1634-80A6-4C14-8B23-456B3549A1D1}">
       <text>
         <r>
           <rPr>
@@ -276,7 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{995594FD-5A68-4BD6-B915-1684D8EE580E}">
+    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{A108287B-3489-417B-9B67-DF09DC020AB2}">
       <text>
         <r>
           <rPr>
@@ -300,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K4" authorId="0" shapeId="0" xr:uid="{60E91CFC-671E-4735-BA0F-A1968A5CA962}">
+    <comment ref="K4" authorId="0" shapeId="0" xr:uid="{AAA7F9E4-18AE-42A6-A2BF-37E9166B1F8B}">
       <text>
         <r>
           <rPr>
@@ -324,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L4" authorId="0" shapeId="0" xr:uid="{8F72F59D-07FE-4932-9FC0-2E70F63EE29D}">
+    <comment ref="L4" authorId="0" shapeId="0" xr:uid="{96FCE090-7A9D-4F3C-9EBE-0AAE265FC45D}">
       <text>
         <r>
           <rPr>
@@ -348,7 +348,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="0" shapeId="0" xr:uid="{D63CE3E4-1B61-44C1-8B9D-7F4E722593CF}">
+    <comment ref="M4" authorId="0" shapeId="0" xr:uid="{6F1BCEBB-F888-4C6D-8810-FF03F7445EB8}">
       <text>
         <r>
           <rPr>
@@ -372,7 +372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N4" authorId="0" shapeId="0" xr:uid="{B9F78EBD-DB8B-4839-BB2A-C6BDD4F47EBF}">
+    <comment ref="N4" authorId="0" shapeId="0" xr:uid="{A36D8C7E-6783-4A56-BA80-1B8B53A3F139}">
       <text>
         <r>
           <rPr>
@@ -396,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{C4ADDAF8-9FBE-4F55-832A-4EB5CE820A1E}">
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{4B9063D9-D297-49FD-8C77-58BF6A5E6D25}">
       <text>
         <r>
           <rPr>
@@ -420,7 +420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{36404776-48C7-4E55-85AF-B01E9FA913F6}">
+    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{77E57465-48C5-44A8-97B3-59B0104F5CCE}">
       <text>
         <r>
           <rPr>
@@ -444,7 +444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{705F9271-1DDD-49E6-BB9A-228D0DE54E7E}">
+    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{257282EA-C2E0-492D-AC30-37C14BD72177}">
       <text>
         <r>
           <rPr>
@@ -1331,7 +1331,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="123">
   <si>
     <t>Tipo Objeto Dominio</t>
   </si>
@@ -1540,9 +1540,6 @@
     <t>¿Qué hago?</t>
   </si>
   <si>
-    <t>Identifica de forma unívoca a cada uno de los residentes de un conjunto residencial.</t>
-  </si>
-  <si>
     <t>Quitar espacios en blanco al inicio, al final, y entre números</t>
   </si>
   <si>
@@ -1555,18 +1552,6 @@
     <t>conjuntoResidencial</t>
   </si>
   <si>
-    <t>texto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre de zona común único </t>
-  </si>
-  <si>
-    <t>No es posible tener más de una zona común con el mismo nombre para el mismo conjunto residencial</t>
-  </si>
-  <si>
-    <t>estaDisponible</t>
-  </si>
-  <si>
     <t>fechaHoraInicio</t>
   </si>
   <si>
@@ -1591,21 +1576,6 @@
     <t>No puede ser mayor a 24</t>
   </si>
   <si>
-    <t>Representa el nombre de una zona común especifica.</t>
-  </si>
-  <si>
-    <t>Representa la descripción que tiene una zona común</t>
-  </si>
-  <si>
-    <t>Representa el número de residentes que pueden ingresar en una zona común.</t>
-  </si>
-  <si>
-    <t>Representa el tiempo de uso permitido por residente de una zona común.</t>
-  </si>
-  <si>
-    <t>Representa el contenido de las normas de una zona común.</t>
-  </si>
-  <si>
     <t>Representa el conjunto residencial dónde está la zona común.</t>
   </si>
   <si>
@@ -1621,30 +1591,9 @@
     <t>dd/MM/aaaa HH:MM dónde dd representa el día, MM representa el mes, aaaa, representa el año, HH representa la hora en formato de 24 horas, MM representa los minutos.</t>
   </si>
   <si>
-    <t>Identifica de forma unívoca a cada una de las agendas.</t>
-  </si>
-  <si>
-    <t>Representa el nombre de una agenda determinada.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Representa el estado de disponibilidad de una agenda. </t>
-  </si>
-  <si>
-    <t>Representa la fecha y hora de inicio de una agenda.</t>
-  </si>
-  <si>
-    <t>Representa la fecha y hora de finalización de una agenda.</t>
-  </si>
-  <si>
-    <t>Representa la zona común a la cual está asociada la agenda</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nombre, fecha inicio y fin único. </t>
   </si>
   <si>
-    <t>No es posible tener un nombre fecha de inicio y finalización igual para una misma zona común.</t>
-  </si>
-  <si>
     <t>horaInicio</t>
   </si>
   <si>
@@ -1654,27 +1603,6 @@
     <t>agenda</t>
   </si>
   <si>
-    <t>Identifica de forma unívoca a cada uno de los turnos.</t>
-  </si>
-  <si>
-    <t>Representa el nombre de un turno determinado.</t>
-  </si>
-  <si>
-    <t>nombreNumeroTurno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Representa el estado de disponibilidad de un turno. </t>
-  </si>
-  <si>
-    <t>Representa la fecha y hora de inicio de un turno.</t>
-  </si>
-  <si>
-    <t>Representa la fecha y hora de finalización de un turno.</t>
-  </si>
-  <si>
-    <t>Representa la agenda a la cual está asociado un turno determinado.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nombre, hora de inicio y fin único. </t>
   </si>
   <si>
@@ -1693,14 +1621,92 @@
     <t>unidadTiempoUso</t>
   </si>
   <si>
-    <t>ConjuntoResidencial</t>
+    <t>Es un dato que hace que cada zona común sea única.</t>
+  </si>
+  <si>
+    <t>Es un dato que representa al nombre de una zona comun.</t>
+  </si>
+  <si>
+    <t>Es un dato que representa el formato de texto de una descripción para la zona común.</t>
+  </si>
+  <si>
+    <t>Entero</t>
+  </si>
+  <si>
+    <t>Es un dato que representa el número de personas que admite una zona común.</t>
+  </si>
+  <si>
+    <t>Este es le dato que representa el tiempo de uso por numero entero de un residente</t>
+  </si>
+  <si>
+    <t>Es un dato que representa la unidad de tiempo de uso de una zona comun para un residente.</t>
+  </si>
+  <si>
+    <t>Es un dato que representa el texto de normas que puede tener la zona común</t>
+  </si>
+  <si>
+    <t>Combinación única 1</t>
+  </si>
+  <si>
+    <t>Nombre de zona común y el conjunto residencial</t>
+  </si>
+  <si>
+    <t>No es posible tener más de una zona común con el mismo nombre para un mismo conjunto residencial.</t>
+  </si>
+  <si>
+    <t>disponibilidad</t>
+  </si>
+  <si>
+    <t>Es un dato que hace que cada agenda residencial sea único.</t>
+  </si>
+  <si>
+    <t>Es un dato que representa la zona común con la que está relacionada la agenda especifica.</t>
+  </si>
+  <si>
+    <t>Este es un dato tipo texto que representa el nombre de como se llama la agenda que se esta programando</t>
+  </si>
+  <si>
+    <t>Este dato es un tipo logico que representa si esta disponible o no la agenda</t>
+  </si>
+  <si>
+    <t>Este dato representa la fecha de hora de inicio en la cual empieza la agenda.</t>
+  </si>
+  <si>
+    <t>Este dato representa la fecha de hora final en la cual finaliza una agenda.</t>
+  </si>
+  <si>
+    <t>Una misma agenda no puede repetirse para la misma zona comun, fecha de inicio y fecha final..</t>
+  </si>
+  <si>
+    <t>numeroTurno</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>Es un dato que hace que cada turno sea único.</t>
+  </si>
+  <si>
+    <t>Este dato representa el nombre y número con el que se va a concoer el turno por defecto la palabra "Turno" y luego un numero consecutivo</t>
+  </si>
+  <si>
+    <t>Es un dato que representa la hora de inicio del turno.</t>
+  </si>
+  <si>
+    <t>Es un dato que representa la hora de finalización del turno.</t>
+  </si>
+  <si>
+    <t>Este dato es de tipo logico el cual dice si esta disponible o no disponible un turno</t>
+  </si>
+  <si>
+    <t>Este dato representa con que agenda está relacionada el turno.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1760,6 +1766,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2172,7 +2185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2361,6 +2374,60 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2397,60 +2464,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2462,6 +2475,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2551,29 +2570,36 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
+      <xxl21:absoluteUrl r:id="rId3"/>
     </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="Objetos de dominio"/>
+      <sheetName val="Valores"/>
+      <sheetName val="Modelo Dominio Anemico Contexto"/>
+      <sheetName val="Listado Objetos Dominio"/>
+      <sheetName val="ConjuntoResidencial"/>
+      <sheetName val="ZonaComun"/>
       <sheetName val="Administrador"/>
-      <sheetName val="ConjuntoResidencial"/>
-      <sheetName val="Zonainmueble"/>
+      <sheetName val="ZonaInmueble"/>
       <sheetName val="Inmueble"/>
-      <sheetName val="ZonaComun"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5">
-        <row r="2">
-          <cell r="G2" t="str">
-            <v>Es un dato que representa la unidad de tiempo de uso de una zona comun para un residente.</v>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>ZonaComun</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y poder usarlos.</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3013,9 +3039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6DC33F5-6024-4ECE-8864-A6190D431B22}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3107,8 +3131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BC2B36-176F-457B-9E5A-2C1354FBA2A7}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3139,73 +3163,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="94" t="str">
-        <f>'Listado Objetos de Dominio'!A3</f>
+      <c r="B2" s="70" t="str">
+        <f>'[1]Listado Objetos Dominio'!A4</f>
         <v>ZonaComun</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="94"/>
-      <c r="P2" s="94"/>
-      <c r="Q2" s="94"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="95" t="str">
-        <f>'Listado Objetos de Dominio'!B3</f>
-        <v>Objeto de dominio que representa a cada una de las zonas comúnes que tendrán una agenda y respectivos turnos.</v>
-      </c>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="95"/>
+      <c r="B3" s="71" t="str">
+        <f>'[1]Listado Objetos Dominio'!B4</f>
+        <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y poder usarlos.</v>
+      </c>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
@@ -3314,7 +3338,7 @@
         <v>52</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="R5" s="27"/>
       <c r="S5" s="28"/>
@@ -3343,7 +3367,7 @@
       </c>
       <c r="J6" s="23"/>
       <c r="K6" s="25" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="L6" s="26" t="s">
         <v>53</v>
@@ -3361,7 +3385,7 @@
         <v>53</v>
       </c>
       <c r="Q6" s="24" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="R6" s="27"/>
       <c r="S6" s="28"/>
@@ -3370,7 +3394,7 @@
     </row>
     <row r="7" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>8</v>
@@ -3390,7 +3414,7 @@
       </c>
       <c r="J7" s="23"/>
       <c r="K7" s="25" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="L7" s="26" t="s">
         <v>53</v>
@@ -3408,7 +3432,7 @@
         <v>53</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="R7" s="27"/>
       <c r="S7" s="28"/>
@@ -3417,10 +3441,10 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
@@ -3429,7 +3453,7 @@
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
       <c r="I8" s="24" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J8" s="23"/>
       <c r="K8" s="23"/>
@@ -3449,7 +3473,7 @@
         <v>53</v>
       </c>
       <c r="Q8" s="24" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="R8" s="27"/>
       <c r="S8" s="28"/>
@@ -3458,10 +3482,10 @@
     </row>
     <row r="9" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
@@ -3470,11 +3494,11 @@
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
       <c r="I9" s="24" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J9" s="23"/>
       <c r="K9" s="25" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L9" s="23" t="s">
         <v>53</v>
@@ -3483,7 +3507,7 @@
         <v>53</v>
       </c>
       <c r="N9" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O9" s="23" t="s">
         <v>53</v>
@@ -3492,26 +3516,22 @@
         <v>53</v>
       </c>
       <c r="Q9" s="24" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="R9" s="27"/>
       <c r="S9" s="28"/>
       <c r="T9" s="29"/>
       <c r="U9" s="30"/>
     </row>
-    <row r="10" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="23">
-        <v>1</v>
-      </c>
-      <c r="D10" s="23">
-        <v>50</v>
-      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
       <c r="G10" s="23"/>
@@ -3520,10 +3540,8 @@
         <v>55</v>
       </c>
       <c r="J10" s="23"/>
-      <c r="K10" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="L10" s="26" t="s">
+      <c r="K10" s="25"/>
+      <c r="L10" s="23" t="s">
         <v>53</v>
       </c>
       <c r="M10" s="23" t="s">
@@ -3538,9 +3556,8 @@
       <c r="P10" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="Q10" s="24" t="str">
-        <f>[1]ZonaComun!$G$2</f>
-        <v>Es un dato que representa la unidad de tiempo de uso de una zona comun para un residente.</v>
+      <c r="Q10" s="24" t="s">
+        <v>102</v>
       </c>
       <c r="R10" s="27"/>
       <c r="S10" s="28"/>
@@ -3549,10 +3566,10 @@
     </row>
     <row r="11" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="C11" s="23">
         <v>1</v>
@@ -3569,7 +3586,7 @@
       </c>
       <c r="J11" s="23"/>
       <c r="K11" s="25" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="L11" s="26" t="s">
         <v>53</v>
@@ -3587,7 +3604,7 @@
         <v>53</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="R11" s="27"/>
       <c r="S11" s="28"/>
@@ -3596,10 +3613,10 @@
     </row>
     <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
@@ -3626,7 +3643,7 @@
         <v>53</v>
       </c>
       <c r="Q12" s="24" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="R12" s="27"/>
       <c r="S12" s="28"/>
@@ -3635,11 +3652,11 @@
     </row>
     <row r="13" spans="1:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="90" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="91"/>
-      <c r="C14" s="92"/>
+      <c r="A14" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="67"/>
+      <c r="C14" s="68"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
@@ -3653,65 +3670,65 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="84" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="86" t="s">
-        <v>76</v>
+      <c r="A16" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="74" t="s">
+        <v>106</v>
       </c>
       <c r="C16" s="35" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="85"/>
-      <c r="B17" s="87"/>
+      <c r="A17" s="73"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="78"/>
-      <c r="C19" s="78" t="s">
+      <c r="B19" s="77"/>
+      <c r="C19" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78" t="s">
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78" t="s">
+      <c r="I19" s="77"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="L19" s="78"/>
-      <c r="M19" s="78"/>
-      <c r="N19" s="78"/>
-      <c r="O19" s="78"/>
-      <c r="P19" s="78" t="s">
+      <c r="L19" s="77"/>
+      <c r="M19" s="77"/>
+      <c r="N19" s="77"/>
+      <c r="O19" s="77"/>
+      <c r="P19" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="Q19" s="78"/>
-      <c r="R19" s="78" t="s">
+      <c r="Q19" s="77"/>
+      <c r="R19" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="S19" s="79"/>
+      <c r="S19" s="80"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="89"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
       <c r="H20" s="37" t="s">
         <v>64</v>
       </c>
@@ -3724,12 +3741,12 @@
       <c r="K20" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="L20" s="80" t="s">
+      <c r="L20" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="80"/>
-      <c r="N20" s="80"/>
-      <c r="O20" s="80"/>
+      <c r="M20" s="79"/>
+      <c r="N20" s="79"/>
+      <c r="O20" s="79"/>
       <c r="P20" s="37" t="s">
         <v>66</v>
       </c>
@@ -3767,69 +3784,69 @@
       <c r="S21" s="39"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="90"/>
       <c r="H22" s="42"/>
       <c r="I22" s="40"/>
       <c r="J22" s="41"/>
       <c r="K22" s="43"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="73"/>
-      <c r="N22" s="73"/>
-      <c r="O22" s="73"/>
+      <c r="L22" s="91"/>
+      <c r="M22" s="91"/>
+      <c r="N22" s="91"/>
+      <c r="O22" s="91"/>
       <c r="P22" s="28"/>
       <c r="Q22" s="44"/>
       <c r="R22" s="44"/>
       <c r="S22" s="45"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="75"/>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="76"/>
+      <c r="B23" s="93"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="94"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="94"/>
       <c r="H23" s="47"/>
       <c r="I23" s="48"/>
       <c r="J23" s="46"/>
       <c r="K23" s="49"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="77"/>
-      <c r="N23" s="77"/>
-      <c r="O23" s="77"/>
+      <c r="L23" s="95"/>
+      <c r="M23" s="95"/>
+      <c r="N23" s="95"/>
+      <c r="O23" s="95"/>
       <c r="P23" s="29"/>
       <c r="Q23" s="50"/>
       <c r="R23" s="50"/>
       <c r="S23" s="51"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="67"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
       <c r="H24" s="53"/>
       <c r="I24" s="54"/>
       <c r="J24" s="52"/>
       <c r="K24" s="53"/>
-      <c r="L24" s="69"/>
-      <c r="M24" s="69"/>
-      <c r="N24" s="69"/>
-      <c r="O24" s="69"/>
+      <c r="L24" s="87"/>
+      <c r="M24" s="87"/>
+      <c r="N24" s="87"/>
+      <c r="O24" s="87"/>
       <c r="P24" s="30"/>
       <c r="Q24" s="55"/>
       <c r="R24" s="55"/>
@@ -3837,18 +3854,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A19:B20"/>
-    <mergeCell ref="C19:G20"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="L20:O20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="C21:G21"/>
     <mergeCell ref="L21:O21"/>
@@ -3862,22 +3867,34 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="L23:O23"/>
+    <mergeCell ref="A19:B20"/>
+    <mergeCell ref="C19:G20"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{A37B2855-ACFA-479C-B06A-FD8440512F11}"/>
-    <hyperlink ref="I24" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{F13992CF-F5F1-4DDC-A387-BCD26ACFBC51}"/>
-    <hyperlink ref="S4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{0EC11F90-A79E-4B65-9D18-7458195FFCB3}"/>
-    <hyperlink ref="T4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{F13F5B8F-A470-43A8-B18B-490DB3960315}"/>
-    <hyperlink ref="U4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{79C534C1-4DBB-44B7-91DC-673B55BE9C76}"/>
-    <hyperlink ref="A22:B22" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{73E8B593-130A-4B51-B491-CBA9818A5291}"/>
-    <hyperlink ref="A21:B21" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{ADFBCBA3-21F7-4DAC-9323-C82903924B4C}"/>
-    <hyperlink ref="A24:B24" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{9B7049B6-504E-4D10-B27F-B6F6A55662CB}"/>
-    <hyperlink ref="R4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{E3D4DA29-2AA5-4D85-86F9-7BF7982D8569}"/>
-    <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{E623D929-425F-430D-84C6-20E89FCA63A8}"/>
-    <hyperlink ref="A23:B23" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{996910C1-B38D-4573-9988-E75C7389CC3A}"/>
-    <hyperlink ref="A5" location="Residente!A12" display="identificador" xr:uid="{0A4FCE87-A9CF-4ED7-8769-A328C8D230AE}"/>
-    <hyperlink ref="C16" location="ZonaComun!A6" display="nombre" xr:uid="{1917D422-53D3-4E12-84AE-0BAFFA848476}"/>
-    <hyperlink ref="C17" location="ZonaComun!A11" display="conjuntoResidencial" xr:uid="{A1BD3261-AA24-49AC-80D8-B62D3C3ECFE9}"/>
+    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{5CF40659-DFE6-490B-8F27-C76F1B381885}"/>
+    <hyperlink ref="I24" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{85CACFD0-E320-4D18-AC58-54D77FBE5DEA}"/>
+    <hyperlink ref="S4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{C3F0C27D-BC9E-448D-9DC8-DC829F7C1493}"/>
+    <hyperlink ref="T4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{D110B68A-00A9-48B9-A57E-B6C7C00FDE89}"/>
+    <hyperlink ref="U4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{3048AD03-22B9-4D07-96D9-012E68BDACCD}"/>
+    <hyperlink ref="A22:B22" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{B4EF5D7B-19B4-4FED-963C-03D71E7A6DE2}"/>
+    <hyperlink ref="A21:B21" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{D152F4FA-BAE8-47AE-9602-FCB10D70E615}"/>
+    <hyperlink ref="A24:B24" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{FAB3C069-1AF5-4561-B78A-8E2C3B3016DC}"/>
+    <hyperlink ref="R4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{C5864519-CEB2-4551-91C7-14CCD6735F74}"/>
+    <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{10212072-64F9-4E47-AEF7-64DC2E58CFB9}"/>
+    <hyperlink ref="A23:B23" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{389BBED9-2A4A-4CED-BCF0-BB55887E5D4A}"/>
+    <hyperlink ref="A5" location="Residente!A12" display="identificador" xr:uid="{E94BA7AD-D3E6-4259-B695-0AEE0A06D04D}"/>
+    <hyperlink ref="C16" location="ZonaComun!A6" display="nombre" xr:uid="{958AA7A2-C258-49FC-93BB-5FEA68A1CF7C}"/>
+    <hyperlink ref="C17" location="ZonaComun!A12" display="conjuntoResidencial" xr:uid="{F39D176D-7AF9-4715-9CF6-B8246E328FE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3889,7 +3906,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3920,73 +3937,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="94" t="str">
+      <c r="B2" s="70" t="str">
         <f>'Listado Objetos de Dominio'!A4</f>
         <v>Agenda</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="94"/>
-      <c r="P2" s="94"/>
-      <c r="Q2" s="94"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="95" t="str">
+      <c r="B3" s="71" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representaa cada una de las agendas que dónde el residente podrá reservar.</v>
       </c>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="95"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
@@ -4075,7 +4092,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="24" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="J5" s="23"/>
       <c r="K5" s="25"/>
@@ -4095,7 +4112,7 @@
         <v>52</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="R5" s="27"/>
       <c r="S5" s="28"/>
@@ -4120,11 +4137,11 @@
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
       <c r="I6" s="24" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="J6" s="23"/>
       <c r="K6" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L6" s="26" t="s">
         <v>53</v>
@@ -4142,7 +4159,7 @@
         <v>53</v>
       </c>
       <c r="Q6" s="24" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="R6" s="27"/>
       <c r="S6" s="28"/>
@@ -4151,10 +4168,10 @@
     </row>
     <row r="7" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>77</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>82</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
@@ -4163,11 +4180,11 @@
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="24" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="J7" s="23"/>
       <c r="K7" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L7" s="26" t="s">
         <v>53</v>
@@ -4185,7 +4202,7 @@
         <v>53</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="R7" s="27"/>
       <c r="S7" s="28"/>
@@ -4194,10 +4211,10 @@
     </row>
     <row r="8" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
@@ -4206,7 +4223,7 @@
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
       <c r="I8" s="24" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J8" s="23"/>
       <c r="K8" s="23"/>
@@ -4226,7 +4243,7 @@
         <v>53</v>
       </c>
       <c r="Q8" s="24" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="R8" s="27"/>
       <c r="S8" s="28"/>
@@ -4235,10 +4252,10 @@
     </row>
     <row r="9" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
@@ -4247,7 +4264,7 @@
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
       <c r="I9" s="24" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J9" s="23"/>
       <c r="K9" s="25"/>
@@ -4267,7 +4284,7 @@
         <v>53</v>
       </c>
       <c r="Q9" s="24" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="R9" s="27"/>
       <c r="S9" s="28"/>
@@ -4275,8 +4292,8 @@
       <c r="U9" s="30"/>
     </row>
     <row r="10" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
-        <v>80</v>
+      <c r="A10" s="100" t="s">
+        <v>75</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>20</v>
@@ -4290,7 +4307,7 @@
       <c r="I10" s="24"/>
       <c r="J10" s="23"/>
       <c r="K10" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L10" s="26" t="s">
         <v>53</v>
@@ -4308,7 +4325,7 @@
         <v>53</v>
       </c>
       <c r="Q10" s="24" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="R10" s="27"/>
       <c r="S10" s="28"/>
@@ -4317,11 +4334,11 @@
     </row>
     <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="90" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="91"/>
-      <c r="C12" s="92"/>
+      <c r="A12" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="67"/>
+      <c r="C12" s="68"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
@@ -4336,10 +4353,10 @@
     </row>
     <row r="14" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="96" t="s">
-        <v>102</v>
-      </c>
-      <c r="B14" s="86" t="s">
-        <v>103</v>
+        <v>86</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>114</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>54</v>
@@ -4349,65 +4366,65 @@
       <c r="A15" s="97"/>
       <c r="B15" s="99"/>
       <c r="C15" s="35" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="97"/>
       <c r="B16" s="99"/>
       <c r="C16" s="35" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="98"/>
-      <c r="B17" s="87"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="58" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="78"/>
-      <c r="C19" s="78" t="s">
+      <c r="B19" s="77"/>
+      <c r="C19" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78" t="s">
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78" t="s">
+      <c r="I19" s="77"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="L19" s="78"/>
-      <c r="M19" s="78"/>
-      <c r="N19" s="78"/>
-      <c r="O19" s="78"/>
-      <c r="P19" s="78" t="s">
+      <c r="L19" s="77"/>
+      <c r="M19" s="77"/>
+      <c r="N19" s="77"/>
+      <c r="O19" s="77"/>
+      <c r="P19" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="Q19" s="78"/>
-      <c r="R19" s="78" t="s">
+      <c r="Q19" s="77"/>
+      <c r="R19" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="S19" s="79"/>
+      <c r="S19" s="80"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="89"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
       <c r="H20" s="37" t="s">
         <v>64</v>
       </c>
@@ -4420,12 +4437,12 @@
       <c r="K20" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="L20" s="80" t="s">
+      <c r="L20" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="80"/>
-      <c r="N20" s="80"/>
-      <c r="O20" s="80"/>
+      <c r="M20" s="79"/>
+      <c r="N20" s="79"/>
+      <c r="O20" s="79"/>
       <c r="P20" s="37" t="s">
         <v>66</v>
       </c>
@@ -4463,69 +4480,69 @@
       <c r="S21" s="39"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="90"/>
       <c r="H22" s="42"/>
       <c r="I22" s="40"/>
       <c r="J22" s="41"/>
       <c r="K22" s="43"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="73"/>
-      <c r="N22" s="73"/>
-      <c r="O22" s="73"/>
+      <c r="L22" s="91"/>
+      <c r="M22" s="91"/>
+      <c r="N22" s="91"/>
+      <c r="O22" s="91"/>
       <c r="P22" s="28"/>
       <c r="Q22" s="44"/>
       <c r="R22" s="44"/>
       <c r="S22" s="45"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="75"/>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="76"/>
+      <c r="B23" s="93"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="94"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="94"/>
       <c r="H23" s="47"/>
       <c r="I23" s="48"/>
       <c r="J23" s="46"/>
       <c r="K23" s="49"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="77"/>
-      <c r="N23" s="77"/>
-      <c r="O23" s="77"/>
+      <c r="L23" s="95"/>
+      <c r="M23" s="95"/>
+      <c r="N23" s="95"/>
+      <c r="O23" s="95"/>
       <c r="P23" s="29"/>
       <c r="Q23" s="50"/>
       <c r="R23" s="50"/>
       <c r="S23" s="51"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="67"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
       <c r="H24" s="53"/>
       <c r="I24" s="54"/>
       <c r="J24" s="52"/>
       <c r="K24" s="53"/>
-      <c r="L24" s="69"/>
-      <c r="M24" s="69"/>
-      <c r="N24" s="69"/>
-      <c r="O24" s="69"/>
+      <c r="L24" s="87"/>
+      <c r="M24" s="87"/>
+      <c r="N24" s="87"/>
+      <c r="O24" s="87"/>
       <c r="P24" s="30"/>
       <c r="Q24" s="55"/>
       <c r="R24" s="55"/>
@@ -4533,6 +4550,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="L22:O22"/>
     <mergeCell ref="R19:S19"/>
     <mergeCell ref="L20:O20"/>
     <mergeCell ref="A1:Q1"/>
@@ -4546,18 +4575,6 @@
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="K19:O19"/>
     <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="L24:O24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{B2E38F92-070F-4A08-9587-748CDC5E3622}"/>
@@ -4572,8 +4589,11 @@
     <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{A433FCFB-EB7E-4AC1-B327-F142BFE13926}"/>
     <hyperlink ref="A23:B23" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{EE6A4ADC-BDF3-4C4F-A105-860D61932111}"/>
     <hyperlink ref="A5" location="Residente!A12" display="identificador" xr:uid="{BA2A2A16-E84E-428F-9B0B-971E1227A3D7}"/>
-    <hyperlink ref="C14" location="ZonaComun!A6" display="nombre" xr:uid="{81C63A09-F9B6-40F1-BA1B-BDA6F509E477}"/>
-    <hyperlink ref="C17" location="ZonaComun!A11" display="conjuntoResidencial" xr:uid="{3EABB89C-5985-47B0-A0EE-49EF08CADABE}"/>
+    <hyperlink ref="C14" location="Agenda!A6" display="nombre" xr:uid="{81C63A09-F9B6-40F1-BA1B-BDA6F509E477}"/>
+    <hyperlink ref="C17" location="Agenda!A10" display="zonaComun" xr:uid="{3EABB89C-5985-47B0-A0EE-49EF08CADABE}"/>
+    <hyperlink ref="C15" location="Agenda!A8" display="fechaHoraInicio" xr:uid="{4E81D5BB-4714-434F-B294-0DDCFCADB9BA}"/>
+    <hyperlink ref="C16" location="Agenda!A9" display="fechaHoraFin" xr:uid="{A08A84C4-7908-45F6-B8FF-ECD1DEE6FC83}"/>
+    <hyperlink ref="A10" location="ZonaComun!A1" display="zonaComun" xr:uid="{EE4AFC96-A4A8-4B5C-80CA-D6C0B29F1F3D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4584,15 +4604,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC57795F-B02D-497B-A04E-44BC1D3D4128}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" style="8" customWidth="1"/>
     <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
@@ -4616,73 +4636,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="94" t="str">
+      <c r="B2" s="70" t="str">
         <f>'Listado Objetos de Dominio'!A4</f>
         <v>Agenda</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="94"/>
-      <c r="P2" s="94"/>
-      <c r="Q2" s="94"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="95" t="str">
+      <c r="B3" s="71" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representaa cada una de las agendas que dónde el residente podrá reservar.</v>
       </c>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="95"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
@@ -4771,7 +4791,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="24" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="J5" s="23"/>
       <c r="K5" s="25"/>
@@ -4791,7 +4811,7 @@
         <v>52</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="R5" s="27"/>
       <c r="S5" s="28"/>
@@ -4800,7 +4820,7 @@
     </row>
     <row r="6" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>8</v>
@@ -4816,11 +4836,11 @@
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
       <c r="I6" s="24" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="J6" s="23"/>
       <c r="K6" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L6" s="26" t="s">
         <v>53</v>
@@ -4838,19 +4858,19 @@
         <v>53</v>
       </c>
       <c r="Q6" s="24" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="R6" s="27"/>
       <c r="S6" s="28"/>
       <c r="T6" s="29"/>
       <c r="U6" s="30"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
@@ -4859,10 +4879,10 @@
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="24" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J7" s="23"/>
-      <c r="K7" s="25"/>
+      <c r="K7" s="23"/>
       <c r="L7" s="26" t="s">
         <v>53</v>
       </c>
@@ -4879,7 +4899,7 @@
         <v>53</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="R7" s="27"/>
       <c r="S7" s="28"/>
@@ -4888,10 +4908,10 @@
     </row>
     <row r="8" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
@@ -4900,11 +4920,11 @@
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
       <c r="I8" s="24" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="26" t="s">
+      <c r="K8" s="25"/>
+      <c r="L8" s="23" t="s">
         <v>53</v>
       </c>
       <c r="M8" s="23" t="s">
@@ -4920,19 +4940,19 @@
         <v>53</v>
       </c>
       <c r="Q8" s="24" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="R8" s="27"/>
       <c r="S8" s="28"/>
       <c r="T8" s="29"/>
       <c r="U8" s="30"/>
     </row>
-    <row r="9" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
@@ -4941,11 +4961,11 @@
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
       <c r="I9" s="24" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="J9" s="23"/>
       <c r="K9" s="25"/>
-      <c r="L9" s="23" t="s">
+      <c r="L9" s="26" t="s">
         <v>53</v>
       </c>
       <c r="M9" s="23" t="s">
@@ -4961,7 +4981,7 @@
         <v>53</v>
       </c>
       <c r="Q9" s="24" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="R9" s="27"/>
       <c r="S9" s="28"/>
@@ -4969,8 +4989,8 @@
       <c r="U9" s="30"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
-        <v>106</v>
+      <c r="A10" s="101" t="s">
+        <v>89</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>21</v>
@@ -5000,7 +5020,7 @@
         <v>53</v>
       </c>
       <c r="Q10" s="24" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="R10" s="27"/>
       <c r="S10" s="28"/>
@@ -5009,11 +5029,11 @@
     </row>
     <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="90" t="s">
+      <c r="A12" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="91"/>
-      <c r="C12" s="92"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="68"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
@@ -5028,78 +5048,78 @@
     </row>
     <row r="14" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="96" t="s">
-        <v>114</v>
-      </c>
-      <c r="B14" s="86" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="35" t="s">
         <v>115</v>
-      </c>
-      <c r="C14" s="35" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="97"/>
       <c r="B15" s="99"/>
       <c r="C15" s="35" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="97"/>
       <c r="B16" s="99"/>
       <c r="C16" s="35" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="98"/>
-      <c r="B17" s="87"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="58" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="78"/>
-      <c r="C19" s="78" t="s">
+      <c r="B19" s="77"/>
+      <c r="C19" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78" t="s">
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78" t="s">
+      <c r="I19" s="77"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="L19" s="78"/>
-      <c r="M19" s="78"/>
-      <c r="N19" s="78"/>
-      <c r="O19" s="78"/>
-      <c r="P19" s="78" t="s">
+      <c r="L19" s="77"/>
+      <c r="M19" s="77"/>
+      <c r="N19" s="77"/>
+      <c r="O19" s="77"/>
+      <c r="P19" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="Q19" s="78"/>
-      <c r="R19" s="78" t="s">
+      <c r="Q19" s="77"/>
+      <c r="R19" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="S19" s="79"/>
+      <c r="S19" s="80"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="89"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
       <c r="H20" s="37" t="s">
         <v>64</v>
       </c>
@@ -5112,12 +5132,12 @@
       <c r="K20" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="L20" s="80" t="s">
+      <c r="L20" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="80"/>
-      <c r="N20" s="80"/>
-      <c r="O20" s="80"/>
+      <c r="M20" s="79"/>
+      <c r="N20" s="79"/>
+      <c r="O20" s="79"/>
       <c r="P20" s="37" t="s">
         <v>66</v>
       </c>
@@ -5155,69 +5175,69 @@
       <c r="S21" s="39"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="90"/>
       <c r="H22" s="42"/>
       <c r="I22" s="40"/>
       <c r="J22" s="41"/>
       <c r="K22" s="43"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="73"/>
-      <c r="N22" s="73"/>
-      <c r="O22" s="73"/>
+      <c r="L22" s="91"/>
+      <c r="M22" s="91"/>
+      <c r="N22" s="91"/>
+      <c r="O22" s="91"/>
       <c r="P22" s="28"/>
       <c r="Q22" s="44"/>
       <c r="R22" s="44"/>
       <c r="S22" s="45"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="75"/>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="76"/>
+      <c r="B23" s="93"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="94"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="94"/>
       <c r="H23" s="47"/>
       <c r="I23" s="48"/>
       <c r="J23" s="46"/>
       <c r="K23" s="49"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="77"/>
-      <c r="N23" s="77"/>
-      <c r="O23" s="77"/>
+      <c r="L23" s="95"/>
+      <c r="M23" s="95"/>
+      <c r="N23" s="95"/>
+      <c r="O23" s="95"/>
       <c r="P23" s="29"/>
       <c r="Q23" s="50"/>
       <c r="R23" s="50"/>
       <c r="S23" s="51"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="67"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
       <c r="H24" s="53"/>
       <c r="I24" s="54"/>
       <c r="J24" s="52"/>
       <c r="K24" s="53"/>
-      <c r="L24" s="69"/>
-      <c r="M24" s="69"/>
-      <c r="N24" s="69"/>
-      <c r="O24" s="69"/>
+      <c r="L24" s="87"/>
+      <c r="M24" s="87"/>
+      <c r="N24" s="87"/>
+      <c r="O24" s="87"/>
       <c r="P24" s="30"/>
       <c r="Q24" s="55"/>
       <c r="R24" s="55"/>
@@ -5225,6 +5245,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="L22:O22"/>
     <mergeCell ref="R19:S19"/>
     <mergeCell ref="L20:O20"/>
     <mergeCell ref="A1:Q1"/>
@@ -5238,18 +5270,6 @@
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="K19:O19"/>
     <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="L24:O24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{186E73A2-C89F-4A82-8727-EBDE505719F2}"/>
@@ -5264,10 +5284,11 @@
     <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{29FA51F4-EA75-465F-B83D-77C0A7AEBB70}"/>
     <hyperlink ref="A23:B23" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{405F90EE-26D2-4FCC-AF8D-6B762EC7AB51}"/>
     <hyperlink ref="A5" location="Residente!A12" display="identificador" xr:uid="{A6A4F685-442F-4729-AC02-D8113D7D7CD3}"/>
-    <hyperlink ref="C14" location="ZonaComun!A6" display="nombre" xr:uid="{48090BA0-F21A-47C5-A5EF-2E455DA15E97}"/>
-    <hyperlink ref="C17" location="ZonaComun!A10" display="agenda " xr:uid="{CAC6B7DD-46E4-4767-B6A9-5932EE1449CE}"/>
-    <hyperlink ref="C15" location="Turno!A8" display="horaInicio" xr:uid="{34BE5899-952C-4E04-BCEC-5A73E810002A}"/>
-    <hyperlink ref="C16" location="Turno!A9" display="horaFin" xr:uid="{78281774-F31B-4016-8878-A33140E8F5C7}"/>
+    <hyperlink ref="C14" location="Turno!A6" display="nombreNumeroTurno" xr:uid="{48090BA0-F21A-47C5-A5EF-2E455DA15E97}"/>
+    <hyperlink ref="C17" location="Turno!A10" display="agenda " xr:uid="{CAC6B7DD-46E4-4767-B6A9-5932EE1449CE}"/>
+    <hyperlink ref="C15" location="Turno!A7" display="horaInicio" xr:uid="{34BE5899-952C-4E04-BCEC-5A73E810002A}"/>
+    <hyperlink ref="C16" location="Turno!A8" display="horaFin" xr:uid="{78281774-F31B-4016-8878-A33140E8F5C7}"/>
+    <hyperlink ref="A10" location="Agenda!A1" display="agenda" xr:uid="{DF48106B-3834-41B6-8EA8-ACE88696EA68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Organizando el enriquesido de reservas segun nuestro muestreo de datos
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Modelos de Dominio Enriquecidos/Modelo De Dominio Enriquecido Agendas.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Modelos de Dominio Enriquecidos/Modelo De Dominio Enriquecido Agendas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josez\Documents\Universidad IngeSistemas\Diseño Orientado a Objetos(DOO)\VictusProyect\victus-doc\Doo-Doc\Nueva Version Victus\Modelos de Dominio Enriquecidos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Nueva Version Victus\Modelos de Dominio Enriquecidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A008BD63-2E2D-4E82-97FA-DCA88F8CD5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFE4CD6-65BD-48D1-9826-154FF86CC4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="3" activeTab="5" xr2:uid="{9E75F319-B909-453D-9AFC-FA9C5B40B20E}"/>
+    <workbookView xWindow="10935" yWindow="3390" windowWidth="28800" windowHeight="15285" firstSheet="2" activeTab="5" xr2:uid="{9E75F319-B909-453D-9AFC-FA9C5B40B20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,6 @@
     <sheet name="Agenda" sheetId="5" r:id="rId5"/>
     <sheet name="Turno" sheetId="6" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId7"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1331,7 +1328,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="124">
   <si>
     <t>Tipo Objeto Dominio</t>
   </si>
@@ -1603,12 +1600,6 @@
     <t>agenda</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombre, hora de inicio y fin único. </t>
-  </si>
-  <si>
-    <t>No es posible tener un nombre hora de inicio y finalización igual para una misma agenda.</t>
-  </si>
-  <si>
     <t xml:space="preserve">agenda </t>
   </si>
   <si>
@@ -1700,6 +1691,15 @@
   </si>
   <si>
     <t>Este dato representa con que agenda está relacionada el turno.</t>
+  </si>
+  <si>
+    <t>ConjuntoResidencial</t>
+  </si>
+  <si>
+    <t>No es posible tener un nombre con la misma agenda para la misma hora de inicio y hora final del turno para una misma turno.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre,agenda, hora de inicio y fin único. </t>
   </si>
 </sst>
 </file>
@@ -1831,7 +1831,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -2180,12 +2180,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2353,6 +2379,15 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2374,6 +2409,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2393,10 +2437,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2404,83 +2448,68 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="26" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2564,45 +2593,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId3"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Valores"/>
-      <sheetName val="Modelo Dominio Anemico Contexto"/>
-      <sheetName val="Listado Objetos Dominio"/>
-      <sheetName val="ConjuntoResidencial"/>
-      <sheetName val="ZonaComun"/>
-      <sheetName val="Administrador"/>
-      <sheetName val="ZonaInmueble"/>
-      <sheetName val="Inmueble"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>ZonaComun</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y poder usarlos.</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2928,19 +2918,19 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="63"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2948,7 +2938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -2956,7 +2946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -2964,52 +2954,52 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -3028,7 +3018,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3039,28 +3029,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6DC33F5-6024-4ECE-8864-A6190D431B22}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.44140625" style="8"/>
+    <col min="1" max="1" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="62"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C1" s="64"/>
+      <c r="D1" s="65"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
@@ -3074,7 +3066,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>20</v>
       </c>
@@ -3084,12 +3076,12 @@
       <c r="C3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="63" t="str">
+      <c r="D3" s="66" t="str">
         <f>$B$1</f>
         <v>Agendas</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>21</v>
       </c>
@@ -3099,9 +3091,9 @@
       <c r="C4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="64"/>
-    </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D4" s="67"/>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>22</v>
       </c>
@@ -3111,7 +3103,7 @@
       <c r="C5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="65"/>
+      <c r="D5" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3129,109 +3121,109 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BC2B36-176F-457B-9E5A-2C1354FBA2A7}">
-  <dimension ref="A1:U24"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="8"/>
+    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="70" t="str">
-        <f>'[1]Listado Objetos Dominio'!A4</f>
+      <c r="B2" s="76" t="str">
+        <f>'Listado Objetos de Dominio'!A3</f>
         <v>ZonaComun</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76"/>
+    </row>
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="71" t="str">
-        <f>'[1]Listado Objetos Dominio'!B4</f>
-        <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y poder usarlos.</v>
-      </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="71"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B3" s="77" t="str">
+        <f>'Listado Objetos de Dominio'!B3</f>
+        <v>Objeto de dominio que representa a cada una de las zonas comúnes que tendrán una agenda y respectivos turnos.</v>
+      </c>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>30</v>
       </c>
@@ -3300,7 +3292,7 @@
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>50</v>
       </c>
@@ -3338,14 +3330,14 @@
         <v>52</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R5" s="27"/>
       <c r="S5" s="28"/>
       <c r="T5" s="29"/>
       <c r="U5" s="30"/>
     </row>
-    <row r="6" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>54</v>
       </c>
@@ -3385,14 +3377,14 @@
         <v>53</v>
       </c>
       <c r="Q6" s="24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R6" s="27"/>
       <c r="S6" s="28"/>
       <c r="T6" s="29"/>
       <c r="U6" s="30"/>
     </row>
-    <row r="7" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>70</v>
       </c>
@@ -3432,19 +3424,19 @@
         <v>53</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R7" s="27"/>
       <c r="S7" s="28"/>
       <c r="T7" s="29"/>
       <c r="U7" s="30"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
@@ -3473,19 +3465,19 @@
         <v>53</v>
       </c>
       <c r="Q8" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R8" s="27"/>
       <c r="S8" s="28"/>
       <c r="T8" s="29"/>
       <c r="U8" s="30"/>
     </row>
-    <row r="9" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="27" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
@@ -3516,16 +3508,16 @@
         <v>53</v>
       </c>
       <c r="Q9" s="24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="R9" s="27"/>
       <c r="S9" s="28"/>
       <c r="T9" s="29"/>
       <c r="U9" s="30"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>8</v>
@@ -3557,14 +3549,14 @@
         <v>53</v>
       </c>
       <c r="Q10" s="24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="R10" s="27"/>
       <c r="S10" s="28"/>
       <c r="T10" s="29"/>
       <c r="U10" s="30"/>
     </row>
-    <row r="11" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>71</v>
       </c>
@@ -3604,19 +3596,19 @@
         <v>53</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="R11" s="27"/>
       <c r="S11" s="28"/>
       <c r="T11" s="29"/>
       <c r="U11" s="30"/>
     </row>
-    <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="57" t="s">
         <v>72</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
@@ -3650,15 +3642,15 @@
       <c r="T12" s="29"/>
       <c r="U12" s="30"/>
     </row>
-    <row r="13" spans="1:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="66" t="s">
-        <v>104</v>
-      </c>
-      <c r="B14" s="67"/>
-      <c r="C14" s="68"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="73"/>
+      <c r="C14" s="74"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>57</v>
       </c>
@@ -3669,66 +3661,66 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="72" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" s="74" t="s">
-        <v>106</v>
+    <row r="16" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="78" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="80" t="s">
+        <v>104</v>
       </c>
       <c r="C16" s="35" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="73"/>
-      <c r="B17" s="75"/>
+    <row r="17" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="79"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="36" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="76" t="s">
+    <row r="18" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="77"/>
-      <c r="C19" s="77" t="s">
+      <c r="B19" s="69"/>
+      <c r="C19" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="77"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="77"/>
-      <c r="G19" s="77"/>
-      <c r="H19" s="77" t="s">
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="77"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="77" t="s">
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="L19" s="77"/>
-      <c r="M19" s="77"/>
-      <c r="N19" s="77"/>
-      <c r="O19" s="77"/>
-      <c r="P19" s="77" t="s">
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="Q19" s="77"/>
-      <c r="R19" s="77" t="s">
+      <c r="Q19" s="69"/>
+      <c r="R19" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="S19" s="80"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="78"/>
-      <c r="B20" s="79"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="79"/>
-      <c r="F20" s="79"/>
-      <c r="G20" s="79"/>
+      <c r="S19" s="70"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="98"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
       <c r="H20" s="37" t="s">
         <v>64</v>
       </c>
@@ -3741,12 +3733,12 @@
       <c r="K20" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="L20" s="79" t="s">
+      <c r="L20" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="79"/>
-      <c r="N20" s="79"/>
-      <c r="O20" s="79"/>
+      <c r="M20" s="71"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="71"/>
       <c r="P20" s="37" t="s">
         <v>66</v>
       </c>
@@ -3760,97 +3752,100 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="81" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="82"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="84"/>
       <c r="H21" s="14"/>
       <c r="I21" s="12"/>
       <c r="J21" s="13"/>
       <c r="K21" s="12"/>
-      <c r="L21" s="83"/>
-      <c r="M21" s="83"/>
-      <c r="N21" s="83"/>
-      <c r="O21" s="83"/>
+      <c r="L21" s="84"/>
+      <c r="M21" s="84"/>
+      <c r="N21" s="84"/>
+      <c r="O21" s="84"/>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
       <c r="R21" s="14"/>
       <c r="S21" s="39"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="88" t="s">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="89"/>
-      <c r="C22" s="90"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
       <c r="H22" s="42"/>
       <c r="I22" s="40"/>
       <c r="J22" s="41"/>
       <c r="K22" s="43"/>
-      <c r="L22" s="91"/>
-      <c r="M22" s="91"/>
-      <c r="N22" s="91"/>
-      <c r="O22" s="91"/>
+      <c r="L22" s="92"/>
+      <c r="M22" s="92"/>
+      <c r="N22" s="92"/>
+      <c r="O22" s="92"/>
       <c r="P22" s="28"/>
       <c r="Q22" s="44"/>
       <c r="R22" s="44"/>
       <c r="S22" s="45"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="92" t="s">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="93"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="94"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="95"/>
+      <c r="G23" s="95"/>
       <c r="H23" s="47"/>
       <c r="I23" s="48"/>
       <c r="J23" s="46"/>
       <c r="K23" s="49"/>
-      <c r="L23" s="95"/>
-      <c r="M23" s="95"/>
-      <c r="N23" s="95"/>
-      <c r="O23" s="95"/>
+      <c r="L23" s="96"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="96"/>
+      <c r="O23" s="96"/>
       <c r="P23" s="29"/>
       <c r="Q23" s="50"/>
       <c r="R23" s="50"/>
       <c r="S23" s="51"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="84" t="s">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="85"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="87"/>
       <c r="H24" s="53"/>
       <c r="I24" s="54"/>
       <c r="J24" s="52"/>
       <c r="K24" s="53"/>
-      <c r="L24" s="87"/>
-      <c r="M24" s="87"/>
-      <c r="N24" s="87"/>
-      <c r="O24" s="87"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="88"/>
+      <c r="N24" s="88"/>
+      <c r="O24" s="88"/>
       <c r="P24" s="30"/>
       <c r="Q24" s="55"/>
       <c r="R24" s="55"/>
       <c r="S24" s="56"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C28" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -3906,106 +3901,106 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="8"/>
+    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="70" t="str">
+      <c r="B2" s="76" t="str">
         <f>'Listado Objetos de Dominio'!A4</f>
         <v>Agenda</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76"/>
+    </row>
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="71" t="str">
+      <c r="B3" s="77" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representaa cada una de las agendas que dónde el residente podrá reservar.</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="71"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>30</v>
       </c>
@@ -4074,7 +4069,7 @@
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>50</v>
       </c>
@@ -4112,14 +4107,14 @@
         <v>52</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="R5" s="27"/>
       <c r="S5" s="28"/>
       <c r="T5" s="29"/>
       <c r="U5" s="30"/>
     </row>
-    <row r="6" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>54</v>
       </c>
@@ -4159,16 +4154,16 @@
         <v>53</v>
       </c>
       <c r="Q6" s="24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="R6" s="27"/>
       <c r="S6" s="28"/>
       <c r="T6" s="29"/>
       <c r="U6" s="30"/>
     </row>
-    <row r="7" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>77</v>
@@ -4202,14 +4197,14 @@
         <v>53</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R7" s="27"/>
       <c r="S7" s="28"/>
       <c r="T7" s="29"/>
       <c r="U7" s="30"/>
     </row>
-    <row r="8" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>73</v>
       </c>
@@ -4243,14 +4238,14 @@
         <v>53</v>
       </c>
       <c r="Q8" s="24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R8" s="27"/>
       <c r="S8" s="28"/>
       <c r="T8" s="29"/>
       <c r="U8" s="30"/>
     </row>
-    <row r="9" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>74</v>
       </c>
@@ -4284,15 +4279,15 @@
         <v>53</v>
       </c>
       <c r="Q9" s="24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="R9" s="27"/>
       <c r="S9" s="28"/>
       <c r="T9" s="29"/>
       <c r="U9" s="30"/>
     </row>
-    <row r="10" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="100" t="s">
+    <row r="10" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="59" t="s">
         <v>75</v>
       </c>
       <c r="B10" s="23" t="s">
@@ -4325,22 +4320,22 @@
         <v>53</v>
       </c>
       <c r="Q10" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R10" s="27"/>
       <c r="S10" s="28"/>
       <c r="T10" s="29"/>
       <c r="U10" s="30"/>
     </row>
-    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="66" t="s">
-        <v>104</v>
-      </c>
-      <c r="B12" s="67"/>
-      <c r="C12" s="68"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="73"/>
+      <c r="C12" s="74"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>57</v>
       </c>
@@ -4351,80 +4346,78 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="96" t="s">
+    <row r="14" spans="1:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="74" t="s">
-        <v>114</v>
-      </c>
-      <c r="C14" s="35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="97"/>
-      <c r="B15" s="99"/>
-      <c r="C15" s="35" t="s">
+      <c r="B14" s="80" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="101" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="97"/>
-      <c r="B16" s="99"/>
+    <row r="15" spans="1:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="99"/>
+      <c r="B15" s="100"/>
+      <c r="C15" s="102"/>
+    </row>
+    <row r="16" spans="1:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="99"/>
+      <c r="B16" s="100"/>
       <c r="C16" s="35" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="98"/>
-      <c r="B17" s="75"/>
+    <row r="17" spans="1:19" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="79"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="58" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="76" t="s">
+    <row r="18" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="77"/>
-      <c r="C19" s="77" t="s">
+      <c r="B19" s="69"/>
+      <c r="C19" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="77"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="77"/>
-      <c r="G19" s="77"/>
-      <c r="H19" s="77" t="s">
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="77"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="77" t="s">
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="L19" s="77"/>
-      <c r="M19" s="77"/>
-      <c r="N19" s="77"/>
-      <c r="O19" s="77"/>
-      <c r="P19" s="77" t="s">
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="Q19" s="77"/>
-      <c r="R19" s="77" t="s">
+      <c r="Q19" s="69"/>
+      <c r="R19" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="S19" s="80"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="78"/>
-      <c r="B20" s="79"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="79"/>
-      <c r="F20" s="79"/>
-      <c r="G20" s="79"/>
+      <c r="S19" s="70"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="98"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
       <c r="H20" s="37" t="s">
         <v>64</v>
       </c>
@@ -4437,12 +4430,12 @@
       <c r="K20" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="L20" s="79" t="s">
+      <c r="L20" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="79"/>
-      <c r="N20" s="79"/>
-      <c r="O20" s="79"/>
+      <c r="M20" s="71"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="71"/>
       <c r="P20" s="37" t="s">
         <v>66</v>
       </c>
@@ -4456,100 +4449,100 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="81" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="82"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="84"/>
       <c r="H21" s="14"/>
       <c r="I21" s="12"/>
       <c r="J21" s="13"/>
       <c r="K21" s="12"/>
-      <c r="L21" s="83"/>
-      <c r="M21" s="83"/>
-      <c r="N21" s="83"/>
-      <c r="O21" s="83"/>
+      <c r="L21" s="84"/>
+      <c r="M21" s="84"/>
+      <c r="N21" s="84"/>
+      <c r="O21" s="84"/>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
       <c r="R21" s="14"/>
       <c r="S21" s="39"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="88" t="s">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="89"/>
-      <c r="C22" s="90"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
       <c r="H22" s="42"/>
       <c r="I22" s="40"/>
       <c r="J22" s="41"/>
       <c r="K22" s="43"/>
-      <c r="L22" s="91"/>
-      <c r="M22" s="91"/>
-      <c r="N22" s="91"/>
-      <c r="O22" s="91"/>
+      <c r="L22" s="92"/>
+      <c r="M22" s="92"/>
+      <c r="N22" s="92"/>
+      <c r="O22" s="92"/>
       <c r="P22" s="28"/>
       <c r="Q22" s="44"/>
       <c r="R22" s="44"/>
       <c r="S22" s="45"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="92" t="s">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="93"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="94"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="95"/>
+      <c r="G23" s="95"/>
       <c r="H23" s="47"/>
       <c r="I23" s="48"/>
       <c r="J23" s="46"/>
       <c r="K23" s="49"/>
-      <c r="L23" s="95"/>
-      <c r="M23" s="95"/>
-      <c r="N23" s="95"/>
-      <c r="O23" s="95"/>
+      <c r="L23" s="96"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="96"/>
+      <c r="O23" s="96"/>
       <c r="P23" s="29"/>
       <c r="Q23" s="50"/>
       <c r="R23" s="50"/>
       <c r="S23" s="51"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="84" t="s">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="85"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="87"/>
       <c r="H24" s="53"/>
       <c r="I24" s="54"/>
       <c r="J24" s="52"/>
       <c r="K24" s="53"/>
-      <c r="L24" s="87"/>
-      <c r="M24" s="87"/>
-      <c r="N24" s="87"/>
-      <c r="O24" s="87"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="88"/>
+      <c r="N24" s="88"/>
+      <c r="O24" s="88"/>
       <c r="P24" s="30"/>
       <c r="Q24" s="55"/>
       <c r="R24" s="55"/>
       <c r="S24" s="56"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="26">
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="L23:O23"/>
@@ -4575,6 +4568,7 @@
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="K19:O19"/>
     <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="C14:C15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{B2E38F92-070F-4A08-9587-748CDC5E3622}"/>
@@ -4589,9 +4583,8 @@
     <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{A433FCFB-EB7E-4AC1-B327-F142BFE13926}"/>
     <hyperlink ref="A23:B23" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{EE6A4ADC-BDF3-4C4F-A105-860D61932111}"/>
     <hyperlink ref="A5" location="Residente!A12" display="identificador" xr:uid="{BA2A2A16-E84E-428F-9B0B-971E1227A3D7}"/>
-    <hyperlink ref="C14" location="Agenda!A6" display="nombre" xr:uid="{81C63A09-F9B6-40F1-BA1B-BDA6F509E477}"/>
     <hyperlink ref="C17" location="Agenda!A10" display="zonaComun" xr:uid="{3EABB89C-5985-47B0-A0EE-49EF08CADABE}"/>
-    <hyperlink ref="C15" location="Agenda!A8" display="fechaHoraInicio" xr:uid="{4E81D5BB-4714-434F-B294-0DDCFCADB9BA}"/>
+    <hyperlink ref="C14" location="Agenda!A8" display="fechaHoraInicio" xr:uid="{4E81D5BB-4714-434F-B294-0DDCFCADB9BA}"/>
     <hyperlink ref="C16" location="Agenda!A9" display="fechaHoraFin" xr:uid="{A08A84C4-7908-45F6-B8FF-ECD1DEE6FC83}"/>
     <hyperlink ref="A10" location="ZonaComun!A1" display="zonaComun" xr:uid="{EE4AFC96-A4A8-4B5C-80CA-D6C0B29F1F3D}"/>
   </hyperlinks>
@@ -4605,106 +4598,106 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="8"/>
+    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="70" t="str">
+      <c r="B2" s="76" t="str">
         <f>'Listado Objetos de Dominio'!A4</f>
         <v>Agenda</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76"/>
+    </row>
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="71" t="str">
+      <c r="B3" s="77" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representaa cada una de las agendas que dónde el residente podrá reservar.</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="71"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>30</v>
       </c>
@@ -4773,7 +4766,7 @@
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>50</v>
       </c>
@@ -4811,16 +4804,16 @@
         <v>52</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="R5" s="27"/>
       <c r="S5" s="28"/>
       <c r="T5" s="29"/>
       <c r="U5" s="30"/>
     </row>
-    <row r="6" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>8</v>
@@ -4858,14 +4851,14 @@
         <v>53</v>
       </c>
       <c r="Q6" s="24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="R6" s="27"/>
       <c r="S6" s="28"/>
       <c r="T6" s="29"/>
       <c r="U6" s="30"/>
     </row>
-    <row r="7" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>87</v>
       </c>
@@ -4899,14 +4892,14 @@
         <v>53</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R7" s="27"/>
       <c r="S7" s="28"/>
       <c r="T7" s="29"/>
       <c r="U7" s="30"/>
     </row>
-    <row r="8" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>88</v>
       </c>
@@ -4940,16 +4933,16 @@
         <v>53</v>
       </c>
       <c r="Q8" s="24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="R8" s="27"/>
       <c r="S8" s="28"/>
       <c r="T8" s="29"/>
       <c r="U8" s="30"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>77</v>
@@ -4981,15 +4974,15 @@
         <v>53</v>
       </c>
       <c r="Q9" s="24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="R9" s="27"/>
       <c r="S9" s="28"/>
       <c r="T9" s="29"/>
       <c r="U9" s="30"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="101" t="s">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="s">
         <v>89</v>
       </c>
       <c r="B10" s="23" t="s">
@@ -5020,22 +5013,22 @@
         <v>53</v>
       </c>
       <c r="Q10" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="R10" s="27"/>
       <c r="S10" s="28"/>
       <c r="T10" s="29"/>
       <c r="U10" s="30"/>
     </row>
-    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="66" t="s">
+    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="67"/>
-      <c r="C12" s="68"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B12" s="73"/>
+      <c r="C12" s="74"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>57</v>
       </c>
@@ -5046,80 +5039,80 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="96" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="74" t="s">
-        <v>91</v>
+    <row r="14" spans="1:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="78" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="80" t="s">
+        <v>122</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="97"/>
-      <c r="B15" s="99"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="99"/>
+      <c r="B15" s="100"/>
       <c r="C15" s="35" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="97"/>
-      <c r="B16" s="99"/>
+    <row r="16" spans="1:21" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="99"/>
+      <c r="B16" s="100"/>
       <c r="C16" s="35" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="98"/>
-      <c r="B17" s="75"/>
+    <row r="17" spans="1:19" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="79"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="58" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="76" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="77"/>
-      <c r="C19" s="77" t="s">
+      <c r="B19" s="69"/>
+      <c r="C19" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="77"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="77"/>
-      <c r="G19" s="77"/>
-      <c r="H19" s="77" t="s">
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="77"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="77" t="s">
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="L19" s="77"/>
-      <c r="M19" s="77"/>
-      <c r="N19" s="77"/>
-      <c r="O19" s="77"/>
-      <c r="P19" s="77" t="s">
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="Q19" s="77"/>
-      <c r="R19" s="77" t="s">
+      <c r="Q19" s="69"/>
+      <c r="R19" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="S19" s="80"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="78"/>
-      <c r="B20" s="79"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="79"/>
-      <c r="F20" s="79"/>
-      <c r="G20" s="79"/>
+      <c r="S19" s="70"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="98"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
       <c r="H20" s="37" t="s">
         <v>64</v>
       </c>
@@ -5132,12 +5125,12 @@
       <c r="K20" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="L20" s="79" t="s">
+      <c r="L20" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="79"/>
-      <c r="N20" s="79"/>
-      <c r="O20" s="79"/>
+      <c r="M20" s="71"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="71"/>
       <c r="P20" s="37" t="s">
         <v>66</v>
       </c>
@@ -5151,93 +5144,93 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="81" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="82"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="84"/>
       <c r="H21" s="14"/>
       <c r="I21" s="12"/>
       <c r="J21" s="13"/>
       <c r="K21" s="12"/>
-      <c r="L21" s="83"/>
-      <c r="M21" s="83"/>
-      <c r="N21" s="83"/>
-      <c r="O21" s="83"/>
+      <c r="L21" s="84"/>
+      <c r="M21" s="84"/>
+      <c r="N21" s="84"/>
+      <c r="O21" s="84"/>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
       <c r="R21" s="14"/>
       <c r="S21" s="39"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="88" t="s">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="89"/>
-      <c r="C22" s="90"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
       <c r="H22" s="42"/>
       <c r="I22" s="40"/>
       <c r="J22" s="41"/>
       <c r="K22" s="43"/>
-      <c r="L22" s="91"/>
-      <c r="M22" s="91"/>
-      <c r="N22" s="91"/>
-      <c r="O22" s="91"/>
+      <c r="L22" s="92"/>
+      <c r="M22" s="92"/>
+      <c r="N22" s="92"/>
+      <c r="O22" s="92"/>
       <c r="P22" s="28"/>
       <c r="Q22" s="44"/>
       <c r="R22" s="44"/>
       <c r="S22" s="45"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="92" t="s">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="93"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="94"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="95"/>
+      <c r="G23" s="95"/>
       <c r="H23" s="47"/>
       <c r="I23" s="48"/>
       <c r="J23" s="46"/>
       <c r="K23" s="49"/>
-      <c r="L23" s="95"/>
-      <c r="M23" s="95"/>
-      <c r="N23" s="95"/>
-      <c r="O23" s="95"/>
+      <c r="L23" s="96"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="96"/>
+      <c r="O23" s="96"/>
       <c r="P23" s="29"/>
       <c r="Q23" s="50"/>
       <c r="R23" s="50"/>
       <c r="S23" s="51"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="84" t="s">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="85"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="87"/>
       <c r="H24" s="53"/>
       <c r="I24" s="54"/>
       <c r="J24" s="52"/>
       <c r="K24" s="53"/>
-      <c r="L24" s="87"/>
-      <c r="M24" s="87"/>
-      <c r="N24" s="87"/>
-      <c r="O24" s="87"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="88"/>
+      <c r="N24" s="88"/>
+      <c r="O24" s="88"/>
       <c r="P24" s="30"/>
       <c r="Q24" s="55"/>
       <c r="R24" s="55"/>

</xml_diff>